<commit_message>
Group review after review meeting
</commit_message>
<xml_diff>
--- a/Group_7_Review.xlsx
+++ b/Group_7_Review.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4DB114E44117BA4C33AC94B1D6D024683EDF37" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0FF6C9B1-2440-4AF1-9EC9-13167D86307B}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="11_AD4DB114E44117BA4C33AC94B1D6D024683EDF37" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1ADE0DD5-5377-452B-B6E6-99322208FE0F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -75,6 +75,144 @@
   </si>
   <si>
     <t>Line#</t>
+  </si>
+  <si>
+    <t>39f</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>function calls should not be inside of if-statement. This practice contradicts on agreed Linux-coding rules</t>
+  </si>
+  <si>
+    <t>Should not use Gloabal variables</t>
+  </si>
+  <si>
+    <t>CodingRules</t>
+  </si>
+  <si>
+    <t>moved function call</t>
+  </si>
+  <si>
+    <t>moved inside classes</t>
+  </si>
+  <si>
+    <t>curly braces indentatition not acording to coding rules</t>
+  </si>
+  <si>
+    <t>changed braces for better readability</t>
+  </si>
+  <si>
+    <t>59f</t>
+  </si>
+  <si>
+    <t>63f</t>
+  </si>
+  <si>
+    <t>try to avoid using exit</t>
+  </si>
+  <si>
+    <t>used return instead</t>
+  </si>
+  <si>
+    <t>main function needs to have a return value</t>
+  </si>
+  <si>
+    <t>used int as return value</t>
+  </si>
+  <si>
+    <t>RuntimeError</t>
+  </si>
+  <si>
+    <t>put sensible variable declarations first in declaration</t>
+  </si>
+  <si>
+    <t>changed way of declaration</t>
+  </si>
+  <si>
+    <t>Readability</t>
+  </si>
+  <si>
+    <t>do not use pointer for confData, is a "wild Pointer"</t>
+  </si>
+  <si>
+    <t>changed to variable, to place in stack or use memory allocation function in heap</t>
+  </si>
+  <si>
+    <t>Memory Management</t>
+  </si>
+  <si>
+    <t>exit should not be used in main loop</t>
+  </si>
+  <si>
+    <t>do not combine two functions together</t>
+  </si>
+  <si>
+    <t>split in open and init function</t>
+  </si>
+  <si>
+    <t>variable name does not tell anything</t>
+  </si>
+  <si>
+    <t>improved name</t>
+  </si>
+  <si>
+    <t>add comment to explain function briefly</t>
+  </si>
+  <si>
+    <t>comment added</t>
+  </si>
+  <si>
+    <t>explain comment</t>
+  </si>
+  <si>
+    <t>added comment to build comment</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>not declared what is defined here</t>
+  </si>
+  <si>
+    <t>added comment</t>
+  </si>
+  <si>
+    <t>every function should have short comment to explain</t>
+  </si>
+  <si>
+    <t>Add author to file</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>added author</t>
+  </si>
+  <si>
+    <t>move function declarations to header file to see easier</t>
+  </si>
+  <si>
+    <t>header file might be needed later</t>
+  </si>
+  <si>
+    <t>explain usage of free parameters</t>
+  </si>
+  <si>
+    <t>add error print to this close function</t>
+  </si>
+  <si>
+    <t>error handling structure added</t>
+  </si>
+  <si>
+    <t>make statement more understandable</t>
+  </si>
+  <si>
+    <t>added normal if-else structure</t>
   </si>
 </sst>
 </file>
@@ -110,8 +248,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -392,194 +533,574 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>266</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>272</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>271</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>318</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>101</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>16</v>
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>194</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1">
+        <v>317</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <v>307</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>